<commit_message>
Kan inte passera sina egna gubbar
Uppdaterat backloggen också
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="80">
   <si>
     <t>Uppgift</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>120+</t>
+  </si>
+  <si>
+    <t>Lapsed triggas när man får en etta och går bakåt motsvarande antal steg.</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G72"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+      <selection activeCell="E73" sqref="E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1448,6 +1451,9 @@
       <c r="B61" t="s">
         <v>5</v>
       </c>
+      <c r="C61" t="s">
+        <v>14</v>
+      </c>
       <c r="D61">
         <v>120</v>
       </c>
@@ -1589,6 +1595,17 @@
       </c>
       <c r="D72" s="2" t="s">
         <v>77</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>79</v>
+      </c>
+      <c r="B73" t="s">
+        <v>5</v>
+      </c>
+      <c r="D73">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Nu kan man slå en sexa!
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="4665"/>
@@ -10,7 +10,6 @@
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="82">
   <si>
     <t>Uppgift</t>
   </si>
@@ -787,7 +786,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -798,7 +797,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A60" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E67" sqref="E67"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1722,12 +1721,18 @@
       <c r="B62" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C62" s="2"/>
+      <c r="C62" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D62" s="2">
         <v>60</v>
       </c>
-      <c r="E62" s="2"/>
-      <c r="F62" s="2"/>
+      <c r="E62" s="2">
+        <v>10</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G62" s="5"/>
       <c r="H62" s="15"/>
       <c r="I62" s="15"/>

</xml_diff>

<commit_message>
Lagt till en kontroll för spärrarna
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="84">
   <si>
     <t>Uppgift</t>
   </si>
@@ -800,7 +800,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -811,7 +811,7 @@
   <dimension ref="A1:K77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1664,12 +1664,18 @@
       <c r="B59" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="2"/>
+      <c r="C59" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="D59" s="2">
         <v>120</v>
       </c>
-      <c r="E59" s="2"/>
-      <c r="F59" s="2"/>
+      <c r="E59" s="2">
+        <v>20</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="G59" s="5"/>
       <c r="H59" s="15"/>
       <c r="I59" s="15"/>

</xml_diff>

<commit_message>
refactoriserat ut message till statistics
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="4665"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="5280"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="86">
   <si>
     <t>Uppgift</t>
   </si>
@@ -271,6 +272,12 @@
   </si>
   <si>
     <t>Fixade en bugg där sexan knuffade bort om en pjäs stod där.</t>
+  </si>
+  <si>
+    <t>Semiklar</t>
+  </si>
+  <si>
+    <t>Uppdaterar inte som den ska... Funkar endast vid första slaget.</t>
   </si>
 </sst>
 </file>
@@ -800,7 +807,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -810,8 +817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -821,7 +828,7 @@
     <col min="3" max="3" width="8.140625" customWidth="1"/>
     <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1901,8 +1908,12 @@
         <v>60</v>
       </c>
       <c r="E69" s="2"/>
-      <c r="F69" s="2"/>
-      <c r="G69" s="5"/>
+      <c r="F69" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>85</v>
+      </c>
       <c r="H69" s="15"/>
       <c r="I69" s="15"/>
       <c r="J69" s="15"/>

</xml_diff>

<commit_message>
finish istället för home och barre uppdaterad
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="98">
   <si>
     <t>Uppgift</t>
   </si>
@@ -280,6 +280,39 @@
   </si>
   <si>
     <t>Lagt in en kontroll som går igenom alla drag en spelare kan göra. Om inga drag kan göras byts turen.</t>
+  </si>
+  <si>
+    <t>Innan vecka 19-20</t>
+  </si>
+  <si>
+    <t>Implementera Gamestate</t>
+  </si>
+  <si>
+    <t>Solitär</t>
+  </si>
+  <si>
+    <t>Move/Förflyttning</t>
+  </si>
+  <si>
+    <t>Regler</t>
+  </si>
+  <si>
+    <t>Spelplan</t>
+  </si>
+  <si>
+    <t>GUI</t>
+  </si>
+  <si>
+    <t>Rapport</t>
+  </si>
+  <si>
+    <t>Multiplayer över nätverk</t>
+  </si>
+  <si>
+    <t>Brainstorma backlog items</t>
+  </si>
+  <si>
+    <t>Setup GIT</t>
   </si>
 </sst>
 </file>
@@ -303,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -328,6 +361,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -515,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -537,6 +588,13 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -809,7 +867,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -817,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K77"/>
+  <dimension ref="A1:K102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A84" sqref="A84"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,1246 +892,1544 @@
     <col min="7" max="7" width="84.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
+      <c r="E3" s="23"/>
+      <c r="F3" s="23"/>
+      <c r="G3" s="23"/>
+    </row>
+    <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B5" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C5" s="25"/>
+      <c r="D5" s="25"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="25"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B8" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="25"/>
+      <c r="D10" s="25"/>
+      <c r="E10" s="25"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="25"/>
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="25"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="25"/>
+      <c r="D13" s="25"/>
+      <c r="E13" s="25"/>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="25" t="s">
+        <v>95</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="25"/>
+      <c r="D14" s="25"/>
+      <c r="E14" s="25"/>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="25"/>
+      <c r="D15" s="25"/>
+      <c r="E15" s="25"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B28" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C28" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D28" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E28" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F28" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G28" s="21" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B30" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C30" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D30" s="20">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E30" s="20">
         <v>20</v>
       </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F30" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="20"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="20" t="s">
         <v>33</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B31" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C31" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D6">
+      <c r="D31" s="20">
         <v>10</v>
       </c>
-      <c r="E6">
+      <c r="E31" s="20">
         <v>15</v>
       </c>
-      <c r="F6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F31" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="20"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B32" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C32" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D7">
+      <c r="D32" s="20">
         <v>60</v>
       </c>
-      <c r="E7">
+      <c r="E32" s="20">
         <v>70</v>
       </c>
-      <c r="F7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F32" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="20"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="20" t="s">
         <v>35</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B33" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C33" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D8">
+      <c r="D33" s="20">
         <v>40</v>
       </c>
-      <c r="E8">
+      <c r="E33" s="20">
         <v>55</v>
       </c>
-      <c r="F8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F33" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="20"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B34" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C34" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D9">
+      <c r="D34" s="20">
         <v>30</v>
       </c>
-      <c r="F9" t="s">
+      <c r="E34" s="20"/>
+      <c r="F34" s="20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G34" s="20"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="20"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
+      <c r="G35" s="20"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="20"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
+      <c r="G36" s="20"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="B37" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D12">
+      <c r="D37" s="20">
         <v>40</v>
       </c>
-      <c r="E12">
+      <c r="E37" s="20">
         <v>30</v>
       </c>
-      <c r="F12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F37" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="20"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="B38" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D13">
+      <c r="D38" s="20">
         <v>10</v>
       </c>
-      <c r="E13">
+      <c r="E38" s="20">
         <v>10</v>
       </c>
-      <c r="F13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F38" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="20"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B39" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C39" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D14">
+      <c r="D39" s="20">
         <v>120</v>
       </c>
-      <c r="E14">
+      <c r="E39" s="20">
         <v>60</v>
       </c>
-      <c r="F14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="F39" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="20"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B40" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C40" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D15">
+      <c r="D40" s="20">
         <v>60</v>
       </c>
-      <c r="E15">
+      <c r="E40" s="20">
         <v>60</v>
       </c>
-      <c r="F15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="F40" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="20"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="B16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B41" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C41" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D16">
+      <c r="D41" s="20">
         <v>20</v>
       </c>
-      <c r="E16">
+      <c r="E41" s="20">
         <v>15</v>
       </c>
-      <c r="F16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="F41" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="20"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B42" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C42" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="F17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="20"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B43" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C43" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D18">
+      <c r="D43" s="20">
         <v>40</v>
       </c>
-      <c r="E18">
+      <c r="E43" s="20">
         <v>30</v>
       </c>
-      <c r="F18" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F43" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="20"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B44" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C44" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D19">
+      <c r="D44" s="20">
         <v>30</v>
       </c>
-      <c r="E19">
+      <c r="E44" s="20">
         <v>30</v>
       </c>
-      <c r="F19" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F44" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G44" s="20"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B45" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C45" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D20">
+      <c r="D45" s="20">
         <v>15</v>
       </c>
-      <c r="E20">
+      <c r="E45" s="20">
         <v>15</v>
       </c>
-      <c r="F20" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F45" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="20"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="20" t="s">
         <v>42</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B46" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C46" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D21">
+      <c r="D46" s="20">
         <v>15</v>
       </c>
-      <c r="E21">
+      <c r="E46" s="20">
         <v>15</v>
       </c>
-      <c r="F21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F46" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="20"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B47" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C47" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D22">
+      <c r="D47" s="20">
         <v>45</v>
       </c>
-      <c r="E22">
+      <c r="E47" s="20">
         <v>30</v>
       </c>
-      <c r="F22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="F47" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="20"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B48" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C48" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D23">
+      <c r="D48" s="20">
         <v>45</v>
       </c>
-      <c r="E23">
+      <c r="E48" s="20">
         <v>30</v>
       </c>
-      <c r="F23" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F48" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="20"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B49" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C49" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D24">
+      <c r="D49" s="20">
         <v>70</v>
       </c>
-      <c r="E24">
+      <c r="E49" s="20">
         <v>60</v>
       </c>
-      <c r="F24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F49" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G49" s="20"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B50" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C50" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D25">
+      <c r="D50" s="20">
         <v>30</v>
       </c>
-      <c r="E25">
+      <c r="E50" s="20">
         <v>20</v>
       </c>
-      <c r="F25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="F50" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="20"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B51" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C51" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D26">
+      <c r="D51" s="20">
         <v>60</v>
       </c>
-      <c r="E26">
+      <c r="E51" s="20">
         <v>45</v>
       </c>
-      <c r="F26" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F51" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G51" s="20"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B52" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C52" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D27">
+      <c r="D52" s="20">
         <v>60</v>
       </c>
-      <c r="E27">
+      <c r="E52" s="20">
         <v>45</v>
       </c>
-      <c r="F27" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="F52" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="20"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B53" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C53" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D28">
+      <c r="D53" s="20">
         <v>45</v>
       </c>
-      <c r="E28">
+      <c r="E53" s="20">
         <v>45</v>
       </c>
-      <c r="F28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="F53" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="20"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="20"/>
+      <c r="B54" s="20"/>
+      <c r="C54" s="20"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
+      <c r="F54" s="20"/>
+      <c r="G54" s="20"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="B30" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B55" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C55" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="F30" t="s">
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
+      <c r="F55" s="20" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="G55" s="20"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B56" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C56" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E31">
+      <c r="D56" s="20"/>
+      <c r="E56" s="20">
         <v>30</v>
       </c>
-      <c r="F31" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="F56" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="20"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="B57" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E32">
+      <c r="D57" s="20"/>
+      <c r="E57" s="20">
         <v>60</v>
       </c>
-      <c r="F32" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="F57" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="20"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B33" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B58" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E33">
+      <c r="D58" s="20"/>
+      <c r="E58" s="20">
         <v>15</v>
       </c>
-      <c r="F33" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="F58" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="20"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B34" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="B59" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C59" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D34">
+      <c r="D59" s="20">
         <v>20</v>
       </c>
-      <c r="E34">
+      <c r="E59" s="20">
         <v>23</v>
       </c>
-      <c r="F34" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F59" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="20"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="B60" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D35">
+      <c r="D60" s="20">
         <v>20</v>
       </c>
-      <c r="E35">
+      <c r="E60" s="20">
         <v>15</v>
       </c>
-      <c r="F35" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="F60" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="20"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="B36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="B61" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1">
+      <c r="D61" s="19"/>
+      <c r="E61" s="19">
         <v>120</v>
       </c>
-      <c r="F36" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="F61" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="20"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="B62" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1">
+      <c r="D62" s="19"/>
+      <c r="E62" s="19">
         <v>60</v>
       </c>
-      <c r="F37" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="F62" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="20"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="B63" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E38">
+      <c r="D63" s="20"/>
+      <c r="E63" s="20">
         <v>30</v>
       </c>
-      <c r="F38" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="F63" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="20"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B64" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E39">
+      <c r="D64" s="20"/>
+      <c r="E64" s="20">
         <v>120</v>
       </c>
-      <c r="F39" t="s">
+      <c r="F64" s="20" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="G64" s="20"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="B40" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B65" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C65" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E40">
+      <c r="D65" s="20"/>
+      <c r="E65" s="20">
         <v>60</v>
       </c>
-      <c r="F40" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="F65" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="20"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="B41" t="s">
-        <v>5</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B66" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C66" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E41">
+      <c r="D66" s="20"/>
+      <c r="E66" s="20">
         <v>75</v>
       </c>
-      <c r="F41" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="F66" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" s="20"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B67" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C67" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E42">
+      <c r="D67" s="20"/>
+      <c r="E67" s="20">
         <v>60</v>
       </c>
-      <c r="F42" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="F67" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="20"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="B68" s="20" t="s">
+        <v>5</v>
+      </c>
+      <c r="C68" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="E43">
+      <c r="D68" s="20"/>
+      <c r="E68" s="20">
         <v>60</v>
       </c>
-      <c r="F43" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+      <c r="F68" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="20"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A69" s="20"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="20"/>
+      <c r="D69" s="20"/>
+      <c r="E69" s="20"/>
+      <c r="F69" s="20"/>
+      <c r="G69" s="20"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B70" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C70" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="D70" s="20"/>
+      <c r="E70" s="20"/>
+      <c r="F70" s="20"/>
+      <c r="G70" s="20"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B71" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C71" s="20" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+      <c r="D71" s="20"/>
+      <c r="E71" s="20"/>
+      <c r="F71" s="20"/>
+      <c r="G71" s="20"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B72" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C72" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="D47">
+      <c r="D72" s="20">
         <v>60</v>
       </c>
-      <c r="E47" t="s">
+      <c r="E72" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="F47" t="s">
+      <c r="F72" s="20" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="G72" s="20"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>30</v>
       </c>
-      <c r="B50" t="s">
-        <v>5</v>
-      </c>
-      <c r="F50" t="s">
+      <c r="B75" t="s">
+        <v>5</v>
+      </c>
+      <c r="F75" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>25</v>
       </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="F51" t="s">
+      <c r="B76" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H56" s="14"/>
-      <c r="I56" s="14"/>
-      <c r="J56" s="14"/>
-      <c r="K56" s="14"/>
-    </row>
-    <row r="57" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="12" t="s">
+    <row r="81" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+    </row>
+    <row r="82" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B82" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C82" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D82" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E82" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F57" s="13" t="s">
+      <c r="F82" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G57" s="16" t="s">
+      <c r="G82" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H57" s="15"/>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="14"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
+      <c r="H82" s="15"/>
+      <c r="I82" s="15"/>
+      <c r="J82" s="15"/>
+      <c r="K82" s="14"/>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A83" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B58" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" s="10" t="s">
+      <c r="B83" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="10">
+      <c r="D83" s="10">
         <v>30</v>
       </c>
-      <c r="E58" s="10">
+      <c r="E83" s="10">
         <v>20</v>
       </c>
-      <c r="F58" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="11"/>
-      <c r="H58" s="15"/>
-      <c r="I58" s="15"/>
-      <c r="J58" s="15"/>
-      <c r="K58" s="14"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" s="4" t="s">
+      <c r="F83" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="11"/>
+      <c r="H83" s="15"/>
+      <c r="I83" s="15"/>
+      <c r="J83" s="15"/>
+      <c r="K83" s="14"/>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A84" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B59" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" s="2" t="s">
+      <c r="B84" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C84" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D84" s="2">
         <v>120</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E84" s="2">
         <v>40</v>
       </c>
-      <c r="F59" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="5"/>
-      <c r="H59" s="15"/>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="14"/>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" s="4" t="s">
+      <c r="F84" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G84" s="5"/>
+      <c r="H84" s="15"/>
+      <c r="I84" s="15"/>
+      <c r="J84" s="15"/>
+      <c r="K84" s="14"/>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B85" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="C85" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D85" s="2">
         <v>30</v>
       </c>
-      <c r="E60" s="2"/>
-      <c r="F60" s="2" t="s">
+      <c r="E85" s="2"/>
+      <c r="F85" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="G60" s="5" t="s">
+      <c r="G85" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H60" s="15"/>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="14"/>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" s="4" t="s">
+      <c r="H85" s="15"/>
+      <c r="I85" s="15"/>
+      <c r="J85" s="15"/>
+      <c r="K85" s="14"/>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A86" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C61" s="2" t="s">
+      <c r="B86" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C86" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D86" s="2">
         <v>120</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E86" s="2">
         <v>20</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="5" t="s">
+      <c r="F86" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G86" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="H61" s="15"/>
-      <c r="I61" s="15"/>
-      <c r="J61" s="15"/>
-      <c r="K61" s="14"/>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="4" t="s">
+      <c r="H86" s="15"/>
+      <c r="I86" s="15"/>
+      <c r="J86" s="15"/>
+      <c r="K86" s="14"/>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A87" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C62" s="2" t="s">
+      <c r="B87" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D87" s="2">
         <v>60</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E87" s="2">
         <v>10</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G62" s="5"/>
-      <c r="H62" s="15"/>
-      <c r="I62" s="15"/>
-      <c r="J62" s="15"/>
-      <c r="K62" s="14"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
+      <c r="F87" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G87" s="5"/>
+      <c r="H87" s="15"/>
+      <c r="I87" s="15"/>
+      <c r="J87" s="15"/>
+      <c r="K87" s="14"/>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A88" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2">
+      <c r="B88" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2">
         <v>100</v>
       </c>
-      <c r="E63" s="2"/>
-      <c r="F63" s="2"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="15"/>
-      <c r="I63" s="15"/>
-      <c r="J63" s="15"/>
-      <c r="K63" s="14"/>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="5"/>
+      <c r="H88" s="15"/>
+      <c r="I88" s="15"/>
+      <c r="J88" s="15"/>
+      <c r="K88" s="14"/>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A89" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2">
+      <c r="B89" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2">
         <v>45</v>
       </c>
-      <c r="E64" s="2"/>
-      <c r="F64" s="2"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="15"/>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="14"/>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" s="4" t="s">
+      <c r="E89" s="2"/>
+      <c r="F89" s="2"/>
+      <c r="G89" s="5"/>
+      <c r="H89" s="15"/>
+      <c r="I89" s="15"/>
+      <c r="J89" s="15"/>
+      <c r="K89" s="14"/>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A90" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B65" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" s="2" t="s">
+      <c r="B90" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C90" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D90" s="2">
         <v>30</v>
       </c>
-      <c r="E65" s="2"/>
-      <c r="F65" s="2"/>
-      <c r="G65" s="5" t="s">
+      <c r="E90" s="2"/>
+      <c r="F90" s="2"/>
+      <c r="G90" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H65" s="15"/>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="14"/>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
+      <c r="H90" s="15"/>
+      <c r="I90" s="15"/>
+      <c r="J90" s="15"/>
+      <c r="K90" s="14"/>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A91" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B91" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C91" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D91" s="2">
         <v>30</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E91" s="2">
         <v>45</v>
       </c>
-      <c r="F66" s="2" t="s">
+      <c r="F91" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="G66" s="5" t="s">
+      <c r="G91" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H66" s="15"/>
-      <c r="I66" s="15"/>
-      <c r="J66" s="15"/>
-      <c r="K66" s="14"/>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" s="4" t="s">
+      <c r="H91" s="15"/>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
+      <c r="K91" s="14"/>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A92" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B92" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="3" t="s">
+      <c r="D92" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E92" s="2">
         <v>15</v>
       </c>
-      <c r="F67" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="5" t="s">
+      <c r="F92" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G92" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="H67" s="15"/>
-      <c r="I67" s="15"/>
-      <c r="J67" s="15"/>
-      <c r="K67" s="14"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="4" t="s">
+      <c r="H92" s="15"/>
+      <c r="I92" s="15"/>
+      <c r="J92" s="15"/>
+      <c r="K92" s="14"/>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A93" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B68" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="3" t="s">
+      <c r="B93" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C93" s="2"/>
+      <c r="D93" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="E68" s="2"/>
-      <c r="F68" s="2"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="15"/>
-      <c r="I68" s="15"/>
-      <c r="J68" s="15"/>
-      <c r="K68" s="14"/>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" s="4" t="s">
+      <c r="E93" s="2"/>
+      <c r="F93" s="2"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="15"/>
+      <c r="I93" s="15"/>
+      <c r="J93" s="15"/>
+      <c r="K93" s="14"/>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A94" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B69" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C69" s="2" t="s">
+      <c r="B94" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C94" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D94" s="2">
         <v>60</v>
       </c>
-      <c r="E69" s="2"/>
-      <c r="F69" s="2" t="s">
+      <c r="E94" s="2"/>
+      <c r="F94" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G69" s="5" t="s">
+      <c r="G94" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="H69" s="15"/>
-      <c r="I69" s="15"/>
-      <c r="J69" s="15"/>
-      <c r="K69" s="14"/>
-    </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" s="4" t="s">
+      <c r="H94" s="15"/>
+      <c r="I94" s="15"/>
+      <c r="J94" s="15"/>
+      <c r="K94" s="14"/>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B70" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="2" t="s">
+      <c r="B95" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C95" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D95" s="2">
         <v>60</v>
       </c>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="15"/>
-      <c r="I70" s="15"/>
-      <c r="J70" s="15"/>
-      <c r="K70" s="14"/>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="E95" s="2"/>
+      <c r="F95" s="2"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="15"/>
+      <c r="I95" s="15"/>
+      <c r="J95" s="15"/>
+      <c r="K95" s="14"/>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A96" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C71" s="2"/>
-      <c r="D71" s="3" t="s">
+      <c r="B96" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C96" s="2"/>
+      <c r="D96" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E71" s="2"/>
-      <c r="F71" s="2"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="15"/>
-      <c r="I71" s="15"/>
-      <c r="J71" s="15"/>
-      <c r="K71" s="14"/>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" s="4" t="s">
+      <c r="E96" s="2"/>
+      <c r="F96" s="2"/>
+      <c r="G96" s="5"/>
+      <c r="H96" s="15"/>
+      <c r="I96" s="15"/>
+      <c r="J96" s="15"/>
+      <c r="K96" s="14"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="2"/>
-      <c r="D72" s="3" t="s">
+      <c r="B97" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C97" s="2"/>
+      <c r="D97" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E72" s="2"/>
-      <c r="F72" s="2"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="15"/>
-      <c r="I72" s="15"/>
-      <c r="J72" s="15"/>
-      <c r="K72" s="14"/>
-    </row>
-    <row r="73" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="6" t="s">
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="15"/>
+      <c r="I97" s="15"/>
+      <c r="J97" s="15"/>
+      <c r="K97" s="14"/>
+    </row>
+    <row r="98" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="7"/>
-      <c r="D73" s="7">
+      <c r="B98" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C98" s="7"/>
+      <c r="D98" s="7">
         <v>30</v>
       </c>
-      <c r="E73" s="7"/>
-      <c r="F73" s="7"/>
-      <c r="G73" s="8"/>
-      <c r="H73" s="15"/>
-      <c r="I73" s="15"/>
-      <c r="J73" s="15"/>
-      <c r="K73" s="14"/>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H74" s="14"/>
-      <c r="I74" s="14"/>
-      <c r="J74" s="14"/>
-      <c r="K74" s="14"/>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" s="17" t="s">
+      <c r="E98" s="7"/>
+      <c r="F98" s="7"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="15"/>
+      <c r="I98" s="15"/>
+      <c r="J98" s="15"/>
+      <c r="K98" s="14"/>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H99" s="14"/>
+      <c r="I99" s="14"/>
+      <c r="J99" s="14"/>
+      <c r="K99" s="14"/>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A100" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="B75" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="18" t="s">
+      <c r="B100" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C100" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D75" s="18">
+      <c r="D100" s="18">
         <v>15</v>
       </c>
-      <c r="E75" s="18">
+      <c r="E100" s="18">
         <v>15</v>
       </c>
-      <c r="F75" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G75" s="18"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" s="17" t="s">
+      <c r="F100" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="G100" s="18"/>
+      <c r="H100" s="14"/>
+      <c r="I100" s="14"/>
+      <c r="J100" s="14"/>
+      <c r="K100" s="14"/>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A101" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="B76" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="18" t="s">
+      <c r="B101" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C101" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D76" s="18">
+      <c r="D101" s="18">
         <v>30</v>
       </c>
-      <c r="E76" s="18">
+      <c r="E101" s="18">
         <v>45</v>
       </c>
-      <c r="F76" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14"/>
-    </row>
-    <row r="77" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="17" t="s">
+      <c r="F101" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="H101" s="14"/>
+      <c r="I101" s="14"/>
+      <c r="J101" s="14"/>
+      <c r="K101" s="14"/>
+    </row>
+    <row r="102" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A102" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="B77" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="17" t="s">
+      <c r="B102" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C102" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="E77" s="17">
+      <c r="E102" s="17">
         <v>100</v>
       </c>
-      <c r="F77" s="17" t="s">
+      <c r="F102" s="17" t="s">
         <v>81</v>
       </c>
     </row>

</xml_diff>

<commit_message>
uppdaterat backlogen och guiButton för Ludo
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2445" windowWidth="14715" windowHeight="5280"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="126">
   <si>
     <t>Uppgift</t>
   </si>
@@ -368,6 +368,30 @@
   </si>
   <si>
     <t>Vecka 17-18</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Lagt in bild och kontroll för att sätta ut målet.</t>
+  </si>
+  <si>
+    <t>Kontroll för att målgång</t>
+  </si>
+  <si>
+    <t>Kontroll för regler vid målrakan.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Vecka 21-22</t>
+  </si>
+  <si>
+    <t>Göra massa tester tester tester.</t>
+  </si>
+  <si>
+    <t>Vid ändring till att skapa listor för alla spelare gick det bytydligt lättare och smidigare.</t>
   </si>
 </sst>
 </file>
@@ -633,7 +657,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -654,7 +678,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -937,7 +960,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -945,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K117"/>
+  <dimension ref="A1:K128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A118" sqref="A118"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G120" sqref="G120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,274 +991,274 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+    <row r="3" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
-      <c r="G4" s="24"/>
+      <c r="C4" s="23"/>
+      <c r="D4" s="23"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
+      <c r="C5" s="24"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="24"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="25" t="s">
+      <c r="A8" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="24"/>
+      <c r="G8" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="25" t="s">
+      <c r="A9" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="24" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="24" t="s">
         <v>92</v>
       </c>
-      <c r="B10" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
+      <c r="B10" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="24"/>
+      <c r="D10" s="24"/>
+      <c r="E10" s="24"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="B11" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
+      <c r="B11" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="25" t="s">
+      <c r="A12" s="24" t="s">
         <v>91</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
+      <c r="B12" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
+      <c r="E12" s="24"/>
+      <c r="F12" s="24"/>
+      <c r="G12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="25" t="s">
+      <c r="A13" s="24" t="s">
         <v>90</v>
       </c>
-      <c r="B13" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
+      <c r="B13" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="25" t="s">
+      <c r="A14" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
-      <c r="E14" s="25"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
+      <c r="B14" s="24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14" s="24"/>
+      <c r="D14" s="24"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="25" t="s">
+      <c r="A15" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="B15" s="25" t="s">
+      <c r="B15" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
-      <c r="E15" s="25"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="24"/>
+      <c r="F15" s="24"/>
+      <c r="G15" s="24"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="26" t="s">
+      <c r="A17" s="25" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="A18" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="21" t="s">
+      <c r="C18" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="21" t="s">
+      <c r="E18" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F18" s="21" t="s">
+      <c r="F18" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="28"/>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B20" s="28"/>
-      <c r="C20" s="28"/>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="27" t="s">
+      <c r="A21" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21" s="28"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="B21" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="27"/>
+      <c r="D21" s="27"/>
+      <c r="E21" s="27"/>
+      <c r="F21" s="27"/>
+      <c r="G21" s="27"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="C22" s="28"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="28"/>
+      <c r="B22" s="27" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1243,274 +1266,274 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="21" t="s">
+      <c r="B25" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="21" t="s">
+      <c r="C25" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F25" s="21" t="s">
+      <c r="F25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G25" s="21" t="s">
+      <c r="G25" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="29"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="28"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="29" t="s">
+      <c r="C27" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G27" s="29"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="28"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G28" s="29"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="28"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="28" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G29" s="29"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="28"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="28" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="28" t="s">
         <v>88</v>
       </c>
-      <c r="C30" s="29" t="s">
+      <c r="C30" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G30" s="29"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="28"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B31" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" s="29" t="s">
+      <c r="B31" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C31" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="29"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G31" s="28"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="B32" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" s="29" t="s">
+      <c r="B32" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="29"/>
+      <c r="D32" s="28"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G32" s="28"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="28" t="s">
         <v>105</v>
       </c>
-      <c r="B33" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C33" s="29" t="s">
+      <c r="B33" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C33" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="29"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="28"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C34" s="29" t="s">
+      <c r="B34" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C34" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="29"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="28"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="B35" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" s="29" t="s">
+      <c r="B35" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C35" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D35" s="29"/>
-      <c r="E35" s="29"/>
-      <c r="F35" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="29"/>
+      <c r="D35" s="28"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="28"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="B36" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="29" t="s">
+      <c r="B36" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C36" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D36" s="29"/>
-      <c r="E36" s="29"/>
-      <c r="F36" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="29"/>
+      <c r="D36" s="28"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="28"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="B37" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" s="29"/>
-      <c r="D37" s="29"/>
-      <c r="E37" s="29"/>
-      <c r="F37" s="29"/>
-      <c r="G37" s="29"/>
+      <c r="B37" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="28"/>
+      <c r="G37" s="28"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="28" t="s">
         <v>110</v>
       </c>
-      <c r="B38" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-      <c r="F38" s="29"/>
-      <c r="G38" s="29"/>
+      <c r="B38" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
+      <c r="G38" s="28"/>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="28" t="s">
         <v>103</v>
       </c>
-      <c r="B39" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" s="29" t="s">
+      <c r="B39" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C39" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-      <c r="F39" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G39" s="29"/>
+      <c r="D39" s="28"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="28"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="B40" s="29" t="s">
-        <v>5</v>
-      </c>
-      <c r="C40" s="29" t="s">
+      <c r="B40" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C40" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D40" s="29"/>
-      <c r="E40" s="29"/>
-      <c r="F40" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="G40" s="29"/>
+      <c r="D40" s="28"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" s="28"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
@@ -1518,847 +1541,847 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="21" t="s">
+      <c r="A43" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="21" t="s">
+      <c r="B43" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="21" t="s">
+      <c r="D43" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F43" s="21" t="s">
+      <c r="F43" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="20" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="20" t="s">
+      <c r="A45" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="20">
+      <c r="D45" s="19">
         <v>10</v>
       </c>
-      <c r="E45" s="20">
+      <c r="E45" s="19">
         <v>20</v>
       </c>
-      <c r="F45" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G45" s="20"/>
+      <c r="F45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G45" s="19"/>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="20" t="s">
+      <c r="A46" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C46" s="20" t="s">
+      <c r="C46" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D46" s="20">
+      <c r="D46" s="19">
         <v>10</v>
       </c>
-      <c r="E46" s="20">
+      <c r="E46" s="19">
         <v>15</v>
       </c>
-      <c r="F46" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="20"/>
+      <c r="F46" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="19"/>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="20">
+      <c r="D47" s="19">
         <v>60</v>
       </c>
-      <c r="E47" s="20">
+      <c r="E47" s="19">
         <v>70</v>
       </c>
-      <c r="F47" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G47" s="20"/>
+      <c r="F47" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G47" s="19"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="20" t="s">
+      <c r="A48" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C48" s="20" t="s">
+      <c r="C48" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D48" s="20">
+      <c r="D48" s="19">
         <v>40</v>
       </c>
-      <c r="E48" s="20">
+      <c r="E48" s="19">
         <v>55</v>
       </c>
-      <c r="F48" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G48" s="20"/>
+      <c r="F48" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G48" s="19"/>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A49" s="20" t="s">
+      <c r="A49" s="19" t="s">
         <v>36</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="20">
+      <c r="D49" s="19">
         <v>30</v>
       </c>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20" t="s">
+      <c r="E49" s="19"/>
+      <c r="F49" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="G49" s="20"/>
+      <c r="G49" s="19"/>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="20"/>
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
+      <c r="A50" s="19"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="20"/>
-      <c r="B51" s="20"/>
-      <c r="C51" s="20"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
-      <c r="G51" s="20"/>
+      <c r="A51" s="19"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="19"/>
+      <c r="D51" s="19"/>
+      <c r="E51" s="19"/>
+      <c r="F51" s="19"/>
+      <c r="G51" s="19"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+      <c r="A52" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B52" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" s="20" t="s">
+      <c r="B52" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C52" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D52" s="20">
+      <c r="D52" s="19">
         <v>40</v>
       </c>
-      <c r="E52" s="20">
+      <c r="E52" s="19">
         <v>30</v>
       </c>
-      <c r="F52" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G52" s="20"/>
+      <c r="F52" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G52" s="19"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="20" t="s">
+      <c r="A53" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C53" s="20" t="s">
+      <c r="B53" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C53" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="20">
+      <c r="D53" s="19">
         <v>10</v>
       </c>
-      <c r="E53" s="20">
+      <c r="E53" s="19">
         <v>10</v>
       </c>
-      <c r="F53" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G53" s="20"/>
+      <c r="F53" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="19"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="20" t="s">
+      <c r="A54" s="19" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C54" s="20" t="s">
+      <c r="C54" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D54" s="20">
+      <c r="D54" s="19">
         <v>120</v>
       </c>
-      <c r="E54" s="20">
+      <c r="E54" s="19">
         <v>60</v>
       </c>
-      <c r="F54" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G54" s="20"/>
+      <c r="F54" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G54" s="19"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="20" t="s">
+      <c r="A55" s="19" t="s">
         <v>20</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D55" s="20">
+      <c r="D55" s="19">
         <v>60</v>
       </c>
-      <c r="E55" s="20">
+      <c r="E55" s="19">
         <v>60</v>
       </c>
-      <c r="F55" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G55" s="20"/>
+      <c r="F55" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G55" s="19"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="20" t="s">
+      <c r="A56" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="B56" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C56" s="20" t="s">
+      <c r="B56" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D56" s="20">
+      <c r="D56" s="19">
         <v>20</v>
       </c>
-      <c r="E56" s="20">
+      <c r="E56" s="19">
         <v>15</v>
       </c>
-      <c r="F56" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G56" s="20"/>
+      <c r="F56" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G56" s="19"/>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="20" t="s">
+      <c r="A57" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B57" s="20" t="s">
+      <c r="B57" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C57" s="20" t="s">
+      <c r="C57" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D57" s="20"/>
-      <c r="E57" s="20"/>
-      <c r="F57" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G57" s="20"/>
+      <c r="D57" s="19"/>
+      <c r="E57" s="19"/>
+      <c r="F57" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" s="19"/>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="20" t="s">
+      <c r="C58" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="20">
+      <c r="D58" s="19">
         <v>40</v>
       </c>
-      <c r="E58" s="20">
+      <c r="E58" s="19">
         <v>30</v>
       </c>
-      <c r="F58" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G58" s="20"/>
+      <c r="F58" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G58" s="19"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="20" t="s">
+      <c r="A59" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C59" s="20" t="s">
+      <c r="C59" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="20">
+      <c r="D59" s="19">
         <v>30</v>
       </c>
-      <c r="E59" s="20">
+      <c r="E59" s="19">
         <v>30</v>
       </c>
-      <c r="F59" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G59" s="20"/>
+      <c r="F59" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G59" s="19"/>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" s="20" t="s">
+      <c r="A60" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B60" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="C60" s="20" t="s">
+      <c r="C60" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D60" s="20">
+      <c r="D60" s="19">
         <v>15</v>
       </c>
-      <c r="E60" s="20">
+      <c r="E60" s="19">
         <v>15</v>
       </c>
-      <c r="F60" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G60" s="20"/>
+      <c r="F60" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G60" s="19"/>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" s="20" t="s">
+      <c r="A61" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D61" s="20">
+      <c r="D61" s="19">
         <v>15</v>
       </c>
-      <c r="E61" s="20">
+      <c r="E61" s="19">
         <v>15</v>
       </c>
-      <c r="F61" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G61" s="20"/>
+      <c r="F61" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" s="19"/>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="20" t="s">
+      <c r="A62" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B62" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C62" s="20" t="s">
+      <c r="C62" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D62" s="20">
+      <c r="D62" s="19">
         <v>45</v>
       </c>
-      <c r="E62" s="20">
+      <c r="E62" s="19">
         <v>30</v>
       </c>
-      <c r="F62" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G62" s="20"/>
+      <c r="F62" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G62" s="19"/>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+      <c r="A63" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B63" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="20">
+      <c r="D63" s="19">
         <v>45</v>
       </c>
-      <c r="E63" s="20">
+      <c r="E63" s="19">
         <v>30</v>
       </c>
-      <c r="F63" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G63" s="20"/>
+      <c r="F63" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G63" s="19"/>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="20" t="s">
+      <c r="A64" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="B64" s="20" t="s">
+      <c r="B64" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D64" s="20">
+      <c r="D64" s="19">
         <v>70</v>
       </c>
-      <c r="E64" s="20">
+      <c r="E64" s="19">
         <v>60</v>
       </c>
-      <c r="F64" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G64" s="20"/>
+      <c r="F64" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G64" s="19"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="20" t="s">
+      <c r="A65" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="B65" s="20" t="s">
+      <c r="B65" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D65" s="20">
+      <c r="D65" s="19">
         <v>30</v>
       </c>
-      <c r="E65" s="20">
+      <c r="E65" s="19">
         <v>20</v>
       </c>
-      <c r="F65" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G65" s="20"/>
+      <c r="F65" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" s="19"/>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
+      <c r="A66" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="B66" s="20" t="s">
+      <c r="B66" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D66" s="20">
+      <c r="D66" s="19">
         <v>60</v>
       </c>
-      <c r="E66" s="20">
+      <c r="E66" s="19">
         <v>45</v>
       </c>
-      <c r="F66" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G66" s="20"/>
+      <c r="F66" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G66" s="19"/>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="20" t="s">
+      <c r="A67" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="B67" s="20" t="s">
+      <c r="B67" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D67" s="20">
+      <c r="D67" s="19">
         <v>60</v>
       </c>
-      <c r="E67" s="20">
+      <c r="E67" s="19">
         <v>45</v>
       </c>
-      <c r="F67" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G67" s="20"/>
+      <c r="F67" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="19"/>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="20" t="s">
+      <c r="A68" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="B68" s="20" t="s">
+      <c r="B68" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D68" s="20">
+      <c r="D68" s="19">
         <v>45</v>
       </c>
-      <c r="E68" s="20">
+      <c r="E68" s="19">
         <v>45</v>
       </c>
-      <c r="F68" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G68" s="20"/>
+      <c r="F68" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G68" s="19"/>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="20"/>
-      <c r="C69" s="20"/>
-      <c r="D69" s="20"/>
-      <c r="E69" s="20"/>
-      <c r="F69" s="20"/>
-      <c r="G69" s="20"/>
+      <c r="A69" s="19"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="19"/>
+      <c r="D69" s="19"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="19"/>
+      <c r="G69" s="19"/>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="20" t="s">
+      <c r="A70" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" s="20" t="s">
+      <c r="B70" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C70" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="20"/>
-      <c r="E70" s="20"/>
-      <c r="F70" s="20" t="s">
+      <c r="D70" s="19"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="G70" s="20"/>
+      <c r="G70" s="19"/>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
+      <c r="A71" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B71" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D71" s="20"/>
-      <c r="E71" s="20">
+      <c r="D71" s="19"/>
+      <c r="E71" s="19">
         <v>30</v>
       </c>
-      <c r="F71" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G71" s="20"/>
+      <c r="F71" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G71" s="19"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="20" t="s">
+      <c r="A72" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="B72" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C72" s="20" t="s">
+      <c r="B72" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C72" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D72" s="20"/>
-      <c r="E72" s="20">
+      <c r="D72" s="19"/>
+      <c r="E72" s="19">
         <v>60</v>
       </c>
-      <c r="F72" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G72" s="20"/>
+      <c r="F72" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G72" s="19"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="20" t="s">
+      <c r="A73" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="B73" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" s="20" t="s">
+      <c r="B73" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C73" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D73" s="20"/>
-      <c r="E73" s="20">
+      <c r="D73" s="19"/>
+      <c r="E73" s="19">
         <v>15</v>
       </c>
-      <c r="F73" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G73" s="20"/>
+      <c r="F73" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G73" s="19"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="20" t="s">
+      <c r="A74" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="B74" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C74" s="20" t="s">
+      <c r="B74" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C74" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D74" s="20">
+      <c r="D74" s="19">
         <v>20</v>
       </c>
-      <c r="E74" s="20">
+      <c r="E74" s="19">
         <v>23</v>
       </c>
-      <c r="F74" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G74" s="20"/>
+      <c r="F74" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G74" s="19"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="20" t="s">
+      <c r="A75" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B75" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C75" s="20" t="s">
+      <c r="B75" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C75" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D75" s="20">
+      <c r="D75" s="19">
         <v>20</v>
       </c>
-      <c r="E75" s="20">
+      <c r="E75" s="19">
         <v>15</v>
       </c>
-      <c r="F75" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G75" s="20"/>
+      <c r="F75" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G75" s="19"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="20" t="s">
+      <c r="A76" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="B76" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C76" s="20" t="s">
+      <c r="B76" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C76" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D76" s="19"/>
-      <c r="E76" s="19">
+      <c r="D76" s="18"/>
+      <c r="E76" s="18">
         <v>120</v>
       </c>
-      <c r="F76" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G76" s="20"/>
+      <c r="F76" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G76" s="19"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="20" t="s">
+      <c r="A77" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="B77" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C77" s="20" t="s">
+      <c r="B77" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C77" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D77" s="19"/>
-      <c r="E77" s="19">
+      <c r="D77" s="18"/>
+      <c r="E77" s="18">
         <v>60</v>
       </c>
-      <c r="F77" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G77" s="20"/>
+      <c r="F77" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G77" s="19"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="20" t="s">
+      <c r="A78" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="B78" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C78" s="20" t="s">
+      <c r="B78" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C78" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="20"/>
-      <c r="E78" s="20">
+      <c r="D78" s="19"/>
+      <c r="E78" s="19">
         <v>30</v>
       </c>
-      <c r="F78" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G78" s="20"/>
+      <c r="F78" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G78" s="19"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
+      <c r="A79" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B79" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C79" s="20" t="s">
+      <c r="B79" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C79" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D79" s="20"/>
-      <c r="E79" s="20">
+      <c r="D79" s="19"/>
+      <c r="E79" s="19">
         <v>120</v>
       </c>
-      <c r="F79" s="20" t="s">
+      <c r="F79" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="G79" s="20"/>
+      <c r="G79" s="19"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="20" t="s">
+      <c r="A80" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="B80" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C80" s="20" t="s">
+      <c r="B80" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C80" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D80" s="20"/>
-      <c r="E80" s="20">
+      <c r="D80" s="19"/>
+      <c r="E80" s="19">
         <v>60</v>
       </c>
-      <c r="F80" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G80" s="20"/>
+      <c r="F80" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G80" s="19"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" s="20" t="s">
+      <c r="A81" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="B81" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="20" t="s">
+      <c r="B81" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D81" s="20"/>
-      <c r="E81" s="20">
+      <c r="D81" s="19"/>
+      <c r="E81" s="19">
         <v>75</v>
       </c>
-      <c r="F81" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G81" s="20"/>
+      <c r="F81" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G81" s="19"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" s="20" t="s">
+      <c r="A82" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B82" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" s="20" t="s">
+      <c r="B82" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C82" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D82" s="20"/>
-      <c r="E82" s="20">
+      <c r="D82" s="19"/>
+      <c r="E82" s="19">
         <v>60</v>
       </c>
-      <c r="F82" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G82" s="20"/>
+      <c r="F82" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G82" s="19"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" s="20" t="s">
+      <c r="A83" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B83" s="20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" s="20" t="s">
+      <c r="B83" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C83" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D83" s="20"/>
-      <c r="E83" s="20">
+      <c r="D83" s="19"/>
+      <c r="E83" s="19">
         <v>60</v>
       </c>
-      <c r="F83" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G83" s="20"/>
+      <c r="F83" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="G83" s="19"/>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" s="20"/>
-      <c r="B84" s="20"/>
-      <c r="C84" s="20"/>
-      <c r="D84" s="20"/>
-      <c r="E84" s="20"/>
-      <c r="F84" s="20"/>
-      <c r="G84" s="20"/>
+      <c r="A84" s="19"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="19"/>
+      <c r="D84" s="19"/>
+      <c r="E84" s="19"/>
+      <c r="F84" s="19"/>
+      <c r="G84" s="19"/>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="20" t="s">
+      <c r="A85" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="B85" s="20" t="s">
+      <c r="B85" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D85" s="20"/>
-      <c r="E85" s="20"/>
-      <c r="F85" s="20"/>
-      <c r="G85" s="20"/>
+      <c r="D85" s="19"/>
+      <c r="E85" s="19"/>
+      <c r="F85" s="19"/>
+      <c r="G85" s="19"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" s="20" t="s">
+      <c r="A86" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="B86" s="20" t="s">
+      <c r="B86" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D86" s="20"/>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="20"/>
+      <c r="D86" s="19"/>
+      <c r="E86" s="19"/>
+      <c r="F86" s="19"/>
+      <c r="G86" s="19"/>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" s="20" t="s">
+      <c r="A87" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="B87" s="20" t="s">
+      <c r="B87" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="D87" s="20">
+      <c r="D87" s="19">
         <v>60</v>
       </c>
-      <c r="E87" s="20" t="s">
+      <c r="E87" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="F87" s="20" t="s">
+      <c r="F87" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G87" s="20"/>
+      <c r="G87" s="19"/>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
@@ -2797,19 +2820,19 @@
       <c r="B115" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C115" s="18" t="s">
+      <c r="C115" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D115" s="18">
+      <c r="D115" s="17">
         <v>15</v>
       </c>
-      <c r="E115" s="18">
+      <c r="E115" s="17">
         <v>15</v>
       </c>
-      <c r="F115" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G115" s="18"/>
+      <c r="F115" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G115" s="17"/>
       <c r="H115" s="14"/>
       <c r="I115" s="14"/>
       <c r="J115" s="14"/>
@@ -2822,18 +2845,19 @@
       <c r="B116" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C116" s="18" t="s">
+      <c r="C116" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D116" s="18">
+      <c r="D116" s="17">
         <v>30</v>
       </c>
-      <c r="E116" s="18">
+      <c r="E116" s="17">
         <v>45</v>
       </c>
-      <c r="F116" s="18" t="s">
-        <v>19</v>
-      </c>
+      <c r="F116" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G116" s="17"/>
       <c r="H116" s="14"/>
       <c r="I116" s="14"/>
       <c r="J116" s="14"/>
@@ -2854,6 +2878,104 @@
       </c>
       <c r="F117" s="17" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A118" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B118" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C118" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" s="17">
+        <v>20</v>
+      </c>
+      <c r="E118" s="17">
+        <v>20</v>
+      </c>
+      <c r="F118" s="17"/>
+      <c r="G118" s="17"/>
+    </row>
+    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A119" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B119" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C119" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D119" s="17"/>
+      <c r="E119" s="17">
+        <v>50</v>
+      </c>
+      <c r="F119" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G119" s="17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A120" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="B120" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C120" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D120" s="17"/>
+      <c r="E120" s="17">
+        <v>400</v>
+      </c>
+      <c r="F120" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G120" s="17"/>
+    </row>
+    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A125" s="25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B127" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C127" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D127" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E127" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="F127" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G127" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Tog en grej i controllrN så nu funkar det nästan.
</commit_message>
<xml_diff>
--- a/BoardGamesG3/Vecka 19 -20.xlsx
+++ b/BoardGamesG3/Vecka 19 -20.xlsx
@@ -960,7 +960,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -968,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K128"/>
+  <dimension ref="A1:AF128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G120" sqref="G120"/>
+    <sheetView tabSelected="1" topLeftCell="B103" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2788,7 +2788,7 @@
       <c r="J112" s="15"/>
       <c r="K112" s="14"/>
     </row>
-    <row r="113" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A113" s="6" t="s">
         <v>79</v>
       </c>
@@ -2807,13 +2807,13 @@
       <c r="J113" s="15"/>
       <c r="K113" s="14"/>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:32" x14ac:dyDescent="0.25">
       <c r="H114" s="14"/>
       <c r="I114" s="14"/>
       <c r="J114" s="14"/>
       <c r="K114" s="14"/>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A115" s="17" t="s">
         <v>82</v>
       </c>
@@ -2838,7 +2838,7 @@
       <c r="J115" s="14"/>
       <c r="K115" s="14"/>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
         <v>83</v>
       </c>
@@ -2863,7 +2863,7 @@
       <c r="J116" s="14"/>
       <c r="K116" s="14"/>
     </row>
-    <row r="117" spans="1:11" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:32" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
         <v>86</v>
       </c>
@@ -2879,8 +2879,33 @@
       <c r="F117" s="17" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H117" s="15"/>
+      <c r="I117" s="15"/>
+      <c r="J117" s="15"/>
+      <c r="K117" s="15"/>
+      <c r="L117" s="15"/>
+      <c r="M117" s="15"/>
+      <c r="N117" s="15"/>
+      <c r="O117" s="15"/>
+      <c r="P117" s="15"/>
+      <c r="Q117" s="15"/>
+      <c r="R117" s="15"/>
+      <c r="S117" s="15"/>
+      <c r="T117" s="15"/>
+      <c r="U117" s="15"/>
+      <c r="V117" s="15"/>
+      <c r="W117" s="15"/>
+      <c r="X117" s="15"/>
+      <c r="Y117" s="15"/>
+      <c r="Z117" s="15"/>
+      <c r="AA117" s="15"/>
+      <c r="AB117" s="15"/>
+      <c r="AC117" s="15"/>
+      <c r="AD117" s="15"/>
+      <c r="AE117" s="15"/>
+      <c r="AF117" s="15"/>
+    </row>
+    <row r="118" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A118" s="17" t="s">
         <v>119</v>
       </c>
@@ -2899,7 +2924,7 @@
       <c r="F118" s="17"/>
       <c r="G118" s="17"/>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A119" s="17" t="s">
         <v>120</v>
       </c>
@@ -2920,7 +2945,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A120" s="17" t="s">
         <v>121</v>
       </c>
@@ -2939,18 +2964,18 @@
       </c>
       <c r="G120" s="17"/>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A125" s="25" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="12" t="s">
         <v>0</v>
       </c>
@@ -2973,7 +2998,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>124</v>
       </c>

</xml_diff>